<commit_message>
upload bahan mentah is clear
</commit_message>
<xml_diff>
--- a/upload/test-data-stock.xlsx
+++ b/upload/test-data-stock.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gladies\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30EB8C0C-429F-4BB5-9A8A-43EAF4AC93B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DB99FA-E08B-224A-8695-E0E92902BE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7518A780-8C7C-49F0-AF96-CB417392CB7C}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15840" xr2:uid="{7518A780-8C7C-49F0-AF96-CB417392CB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Item</t>
   </si>
@@ -69,16 +69,37 @@
   </si>
   <si>
     <t>Ml</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>BM00001</t>
+  </si>
+  <si>
+    <t>BM00002</t>
+  </si>
+  <si>
+    <t>BM00003</t>
+  </si>
+  <si>
+    <t>BM00004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -428,126 +449,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D122A3B-082C-4927-BED4-1515AE1FEEA8}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>44966</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>15000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>150000</v>
       </c>
-      <c r="F2">
-        <f>E2/C2</f>
+      <c r="G2">
+        <f>F2/D2</f>
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>44966</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>10000</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>50000</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F5" si="0">E3/C3</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="0">F3/D3</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>44966</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>8000</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>48000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>44966</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>10000</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>60000</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>